<commit_message>
add working math logic
</commit_message>
<xml_diff>
--- a/Копия ГрафикПрогноз.xlsx
+++ b/Копия ГрафикПрогноз.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Diplom\Diplom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1131FC4E-4758-4647-9C9D-DD02E7F82294}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0324324-17E7-4242-B930-C2E1A8672723}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5C690661-E5AE-4921-AF86-47C106DDCC79}"/>
   </bookViews>
@@ -445,8 +445,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8A82632-FA86-42DE-84B8-EDD4866290F9}" type="CELLRANGE">
-                      <a:rPr lang="ru-RU"/>
+                    <a:fld id="{DF7510C8-23CA-435F-9CE9-5EAC621EB47A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ДИАПАЗОН ЯЧЕЕК]</a:t>
                     </a:fld>
@@ -2849,7 +2849,7 @@
   <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,6 +2989,10 @@
         <f>4.8*A3^3+14.0229*A3^2-1.5029*A3+7.3129</f>
         <v>7.2734122499999998</v>
       </c>
+      <c r="F3">
+        <f ca="1">4.8*C2^3+14.0229*C2^2-1.5029*C2+7.3129</f>
+        <v>7.2739273648452034</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="K3">
         <f t="shared" ref="K3:K51" si="0">K2+J$2</f>
@@ -3024,7 +3028,7 @@
         <v>0.15</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B3:B29" si="1">4.8*A5^3+14.0229*A5^2-1.5029*A5+7.3129</f>
+        <f t="shared" ref="B5:B29" si="1">4.8*A5^3+14.0229*A5^2-1.5029*A5+7.3129</f>
         <v>7.4191802500000001</v>
       </c>
       <c r="I5" s="2"/>

</xml_diff>